<commit_message>
update search bar buttons font
</commit_message>
<xml_diff>
--- a/src/assets/samples/ImportTicketCancellationTemplate.xlsx
+++ b/src/assets/samples/ImportTicketCancellationTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Afaqy\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qasem\OneDrive\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7E131DA2-0168-43D7-8C0E-8F06B5EF972B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C1B47A5F-EAB4-41ED-90F2-D67F22B3C691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F8CF2A45-B278-473C-AD22-2B1052D31D43}"/>
+    <workbookView xWindow="3120" yWindow="720" windowWidth="21975" windowHeight="20880" xr2:uid="{F8CF2A45-B278-473C-AD22-2B1052D31D43}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -392,15 +392,15 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="9.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>